<commit_message>
Updated Time Log and Project Plan
This updates the Project Plan to have COCOMO
model cost estimates for the Planr project.
</commit_message>
<xml_diff>
--- a/Phase 1 Documentation/Phase One Time Log.xlsx
+++ b/Phase 1 Documentation/Phase One Time Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikeblakeman\Desktop\Planr\Planr\Phase 1 Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AB3B3C-F4DE-45D6-8B77-F7BC7FFDD84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED27715-EEA8-4B56-AB83-3BA7B1488495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7715117C-CDDE-9B45-83D9-FB861F637019}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{7715117C-CDDE-9B45-83D9-FB861F637019}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Prototyping UI</t>
+  </si>
+  <si>
+    <t>COCOMO Model for Project Plan.</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -569,7 +572,7 @@
         <v>0.86458333333333337</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" ref="D3:D18" si="0">C3-B3</f>
+        <f t="shared" ref="D3:D19" si="0">C3-B3</f>
         <v>3.125E-2</v>
       </c>
       <c r="E3" t="s">
@@ -889,7 +892,25 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2">
+        <v>44460</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.9458333333333333</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>8.8194444444444464E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -913,9 +934,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1142,27 +1166,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783A39A2-890A-424F-9BFC-50B919DF631D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02DD56A1-62DB-40DA-8A9C-1449A5DCC1EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3897f00b-811b-4797-ad7c-5e248ed43fd2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1ba9b1d7-fc31-4b63-b17e-76a7ddb588b0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1187,9 +1199,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02DD56A1-62DB-40DA-8A9C-1449A5DCC1EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783A39A2-890A-424F-9BFC-50B919DF631D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3897f00b-811b-4797-ad7c-5e248ed43fd2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1ba9b1d7-fc31-4b63-b17e-76a7ddb588b0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>